<commit_message>
Pushing my Lesson Plan for Venv for Robotics Club
</commit_message>
<xml_diff>
--- a/Interview_Projects/SA_Analyst_May_12/311_dict.xlsx
+++ b/Interview_Projects/SA_Analyst_May_12/311_dict.xlsx
@@ -137,8 +137,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">There are Nine Departments: 
-</t>
+      <t xml:space="preserve">There are Nine Departments:
+ </t>
     </r>
     <r>
       <rPr>
@@ -148,10 +148,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">'Animal Care Services', 'Office of Historic Preservation',  
-'Public Works', '311', 'Development Services',  'Parks and Recreation', 'Human Services', 
-'Solid Waste Management', 'Metro Health'
-https://www.sa.gov/Directory/Departments</t>
+      <t xml:space="preserve">'Animal Care Services', 'Office of Historic Preservation',  'Public Works', '311', 'Development Services',  
+'Parks and Recreation', 'Human Services', 'Solid Waste Management', 'Metro Health' </t>
     </r>
   </si>
   <si>
@@ -261,7 +259,9 @@
     <t xml:space="preserve">8 numeric character</t>
   </si>
   <si>
-    <t xml:space="preserve">NAD(1983)State Plane Texas South Central FIPS 4204 Feet </t>
+    <t xml:space="preserve">NAD(1983)State Plane Texas South Central FIPS 4204 Feet 
+Link to NOAA Coordinate Converter
+https://www.ngs.noaa.gov/NCAT/</t>
   </si>
   <si>
     <t xml:space="preserve">YCOORD</t>
@@ -298,7 +298,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +336,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -407,8 +413,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -606,7 +612,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -614,7 +620,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="87.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="88.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="96.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,7 +720,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -803,7 +809,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -813,11 +819,11 @@
       <c r="C16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -861,8 +867,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" display="https://www.sa.gov/Directory/Departments"/>
-    <hyperlink ref="D15" r:id="rId2" display="Council District Map Link:&#10;https://www.sanantonio.gov/Portals/0/Files/GIS/PoliticalMaps/CCD_8.5x11.pdf"/>
+    <hyperlink ref="D15" r:id="rId1" display="Council District Map Link:&#10;https://www.sanantonio.gov/Portals/0/Files/GIS/PoliticalMaps/CCD_8.5x11.pdf"/>
+    <hyperlink ref="D17" r:id="rId2" display="https://www.ngs.noaa.gov/NCAT/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Lots of Good Work done, pushing from the server
</commit_message>
<xml_diff>
--- a/Interview_Projects/SA_Analyst_May_12/311_dict.xlsx
+++ b/Interview_Projects/SA_Analyst_May_12/311_dict.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -54,7 +54,7 @@
       <rPr>
         <b val="true"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -64,7 +64,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -132,7 +132,7 @@
       <rPr>
         <b val="true"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -143,7 +143,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -163,7 +163,7 @@
       <rPr>
         <b val="true"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -174,7 +174,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -211,7 +211,7 @@
       <rPr>
         <b val="true"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -222,7 +222,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -298,10 +298,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -331,16 +331,10 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -392,7 +386,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -413,10 +407,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,201 +419,26 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1f497d"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="eeece1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4f81bd"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="c0504d"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9bbb59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064a2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4bacc6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="f79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ff"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="87.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="96.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="96.38"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -637,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -648,7 +463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -662,7 +477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -673,7 +488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -684,7 +499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -695,7 +510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -709,7 +524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -720,7 +535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -734,7 +549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -748,7 +563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -759,7 +574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -770,7 +585,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -795,7 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -809,7 +624,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="55.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -823,7 +638,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -833,11 +648,11 @@
       <c r="C17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -851,7 +666,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -868,7 +683,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D15" r:id="rId1" display="Council District Map Link:&#10;https://www.sanantonio.gov/Portals/0/Files/GIS/PoliticalMaps/CCD_8.5x11.pdf"/>
-    <hyperlink ref="D17" r:id="rId2" display="https://www.ngs.noaa.gov/NCAT/"/>
+    <hyperlink ref="D17" r:id="rId2" display="NAD(1983)State Plane Texas South Central FIPS 4204 Feet &#10;&#10;Link to NOAA Coordinate Converter&#10;https://www.ngs.noaa.gov/NCAT/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>